<commit_message>
edited L1 scripts for new fmriprep, removed file with backslash in name
</commit_message>
<xml_diff>
--- a/derivatives/covariates/Composite_Reward.xlsx
+++ b/derivatives/covariates/Composite_Reward.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
   <si>
     <t>Subject</t>
   </si>
@@ -44,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -66,11 +66,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -86,6 +88,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -104,13 +108,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
model updated for n = 45
</commit_message>
<xml_diff>
--- a/derivatives/covariates/Composite_Reward.xlsx
+++ b/derivatives/covariates/Composite_Reward.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="3">
   <si>
     <t>Subject</t>
   </si>
@@ -44,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -68,11 +68,13 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -90,6 +92,8 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,13 +112,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -123,494 +127,494 @@
         <v>1001</v>
       </c>
       <c r="B2">
-        <v>-0.61702127659574479</v>
+        <v>-0.62222222222222179</v>
       </c>
       <c r="C2">
-        <v>0.38071525577184262</v>
+        <v>0.38716049382715995</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="B3">
-        <v>-0.61702127659574479</v>
+        <v>-0.62222222222222179</v>
       </c>
       <c r="C3">
-        <v>0.38071525577184262</v>
+        <v>0.38716049382715995</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="B4">
-        <v>2.3829787234042552</v>
+        <v>0.37777777777777821</v>
       </c>
       <c r="C4">
-        <v>5.6785875961973735</v>
+        <v>0.14271604938271637</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="B5">
-        <v>-0.61702127659574479</v>
+        <v>-1.6222222222222218</v>
       </c>
       <c r="C5">
-        <v>0.38071525577184262</v>
+        <v>2.6316049382716034</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="B6">
-        <v>0.38297872340425521</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C6">
-        <v>0.146672702580353</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B7">
-        <v>-1.6170212765957448</v>
+        <v>-4.6222222222222218</v>
       </c>
       <c r="C7">
-        <v>2.6147578089633323</v>
+        <v>21.364938271604935</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B8">
-        <v>2.3829787234042552</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C8">
-        <v>5.6785875961973735</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c r="B9">
-        <v>-4.6170212765957448</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C9">
-        <v>21.316885468537802</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="B10">
-        <v>4.3829787234042552</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C10">
-        <v>19.210502489814395</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c r="B11">
-        <v>-3.6170212765957448</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C11">
-        <v>13.082842915346312</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="B12">
-        <v>2.3829787234042552</v>
+        <v>-1.6222222222222218</v>
       </c>
       <c r="C12">
-        <v>5.6785875961973735</v>
+        <v>2.6316049382716034</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>1019</v>
+        <v>1242</v>
       </c>
       <c r="B13">
-        <v>2.3829787234042552</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C13">
-        <v>5.6785875961973735</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>1021</v>
+        <v>1243</v>
       </c>
       <c r="B14">
-        <v>-1.6170212765957448</v>
+        <v>-2.6222222222222218</v>
       </c>
       <c r="C14">
-        <v>2.6147578089633323</v>
+        <v>6.8760493827160474</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="B15">
-        <v>2.3829787234042552</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C15">
-        <v>5.6785875961973735</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>1243</v>
+        <v>1248</v>
       </c>
       <c r="B16">
-        <v>-2.6170212765957448</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C16">
-        <v>6.8488003621548215</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>1244</v>
+        <v>1249</v>
       </c>
       <c r="B17">
-        <v>4.3829787234042552</v>
+        <v>1.3777777777777782</v>
       </c>
       <c r="C17">
-        <v>19.210502489814395</v>
+        <v>1.8982716049382728</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>1248</v>
+        <v>1251</v>
       </c>
       <c r="B18">
-        <v>2.3829787234042552</v>
+        <v>-4.6222222222222218</v>
       </c>
       <c r="C18">
-        <v>5.6785875961973735</v>
+        <v>21.364938271604935</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>1249</v>
+        <v>1255</v>
       </c>
       <c r="B19">
-        <v>1.3829787234042552</v>
+        <v>-1.6222222222222218</v>
       </c>
       <c r="C19">
-        <v>1.9126301493888633</v>
+        <v>2.6316049382716034</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1251</v>
+        <v>1276</v>
       </c>
       <c r="B20">
-        <v>-4.6170212765957448</v>
+        <v>-2.6222222222222218</v>
       </c>
       <c r="C20">
-        <v>21.316885468537802</v>
+        <v>6.8760493827160474</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>1255</v>
+        <v>1282</v>
       </c>
       <c r="B21">
-        <v>-1.6170212765957448</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C21">
-        <v>2.6147578089633323</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>1276</v>
+        <v>1286</v>
       </c>
       <c r="B22">
-        <v>-2.6170212765957448</v>
+        <v>-0.62222222222222179</v>
       </c>
       <c r="C22">
-        <v>6.8488003621548215</v>
+        <v>0.38716049382715995</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1282</v>
+        <v>1294</v>
       </c>
       <c r="B23">
-        <v>4.3829787234042552</v>
+        <v>-2.6222222222222218</v>
       </c>
       <c r="C23">
-        <v>19.210502489814395</v>
+        <v>6.8760493827160474</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>1286</v>
+        <v>1301</v>
       </c>
       <c r="B24">
-        <v>-0.61702127659574479</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C24">
-        <v>0.38071525577184262</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>1294</v>
+        <v>1302</v>
       </c>
       <c r="B25">
-        <v>-2.6170212765957448</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C25">
-        <v>6.8488003621548215</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="B26">
-        <v>-3.6170212765957448</v>
+        <v>0.37777777777777821</v>
       </c>
       <c r="C26">
-        <v>13.082842915346312</v>
+        <v>0.14271604938271637</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>1302</v>
+        <v>3116</v>
       </c>
       <c r="B27">
-        <v>4.3829787234042552</v>
+        <v>1.3777777777777782</v>
       </c>
       <c r="C27">
-        <v>19.210502489814395</v>
+        <v>1.8982716049382728</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>1303</v>
+        <v>3122</v>
       </c>
       <c r="B28">
-        <v>0.38297872340425521</v>
+        <v>3.3777777777777782</v>
       </c>
       <c r="C28">
-        <v>0.146672702580353</v>
+        <v>11.409382716049386</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>3116</v>
+        <v>3125</v>
       </c>
       <c r="B29">
-        <v>1.3829787234042552</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C29">
-        <v>1.9126301493888633</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>3122</v>
+        <v>3140</v>
       </c>
       <c r="B30">
-        <v>3.3829787234042552</v>
+        <v>-1.6222222222222218</v>
       </c>
       <c r="C30">
-        <v>11.444545043005885</v>
+        <v>2.6316049382716034</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>3125</v>
+        <v>3143</v>
       </c>
       <c r="B31">
-        <v>4.3829787234042552</v>
+        <v>0.37777777777777821</v>
       </c>
       <c r="C31">
-        <v>19.210502489814395</v>
+        <v>0.14271604938271637</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>3140</v>
+        <v>3152</v>
       </c>
       <c r="B32">
-        <v>-1.6170212765957448</v>
+        <v>4.3777777777777782</v>
       </c>
       <c r="C32">
-        <v>2.6147578089633323</v>
+        <v>19.164938271604942</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>3143</v>
+        <v>3166</v>
       </c>
       <c r="B33">
-        <v>0.38297872340425521</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C33">
-        <v>0.146672702580353</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>3152</v>
+        <v>3167</v>
       </c>
       <c r="B34">
-        <v>4.3829787234042552</v>
+        <v>-2.6222222222222218</v>
       </c>
       <c r="C34">
-        <v>19.210502489814395</v>
+        <v>6.8760493827160474</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>3166</v>
+        <v>3170</v>
       </c>
       <c r="B35">
-        <v>-4.6170212765957448</v>
+        <v>-4.6222222222222218</v>
       </c>
       <c r="C35">
-        <v>21.316885468537802</v>
+        <v>21.364938271604935</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>3167</v>
+        <v>3173</v>
       </c>
       <c r="B36">
-        <v>-2.6170212765957448</v>
+        <v>3.3777777777777782</v>
       </c>
       <c r="C36">
-        <v>6.8488003621548215</v>
+        <v>11.409382716049386</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>3170</v>
+        <v>3176</v>
       </c>
       <c r="B37">
-        <v>-4.6170212765957448</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C37">
-        <v>21.316885468537802</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>3173</v>
+        <v>3189</v>
       </c>
       <c r="B38">
-        <v>3.3829787234042552</v>
+        <v>-0.62222222222222179</v>
       </c>
       <c r="C38">
-        <v>11.444545043005885</v>
+        <v>0.38716049382715995</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>3176</v>
+        <v>3190</v>
       </c>
       <c r="B39">
-        <v>-3.6170212765957448</v>
+        <v>3.3777777777777782</v>
       </c>
       <c r="C39">
-        <v>13.082842915346312</v>
+        <v>11.409382716049386</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>3189</v>
+        <v>3199</v>
       </c>
       <c r="B40">
-        <v>-0.61702127659574479</v>
+        <v>0.37777777777777821</v>
       </c>
       <c r="C40">
-        <v>0.38071525577184262</v>
+        <v>0.14271604938271637</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>3190</v>
+        <v>3200</v>
       </c>
       <c r="B41">
-        <v>3.3829787234042552</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C41">
-        <v>11.444545043005885</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>3199</v>
+        <v>3206</v>
       </c>
       <c r="B42">
-        <v>0.38297872340425521</v>
+        <v>-1.6222222222222218</v>
       </c>
       <c r="C42">
-        <v>0.146672702580353</v>
+        <v>2.6316049382716034</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>3200</v>
+        <v>3210</v>
       </c>
       <c r="B43">
-        <v>-3.6170212765957448</v>
+        <v>2.3777777777777782</v>
       </c>
       <c r="C43">
-        <v>13.082842915346312</v>
+        <v>5.6538271604938295</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>3206</v>
+        <v>3212</v>
       </c>
       <c r="B44">
-        <v>-1.6170212765957448</v>
+        <v>-3.6222222222222218</v>
       </c>
       <c r="C44">
-        <v>2.6147578089633323</v>
+        <v>13.120493827160491</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>3210</v>
+        <v>3218</v>
       </c>
       <c r="B45">
-        <v>2.3829787234042552</v>
+        <v>0.37777777777777821</v>
       </c>
       <c r="C45">
-        <v>5.6785875961973735</v>
+        <v>0.14271604938271637</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>3212</v>
+        <v>3220</v>
       </c>
       <c r="B46">
-        <v>-4.6170212765957448</v>
+        <v>1.3777777777777782</v>
       </c>
       <c r="C46">
-        <v>21.316885468537802</v>
+        <v>1.8982716049382728</v>
       </c>
     </row>
     <row r="47">

</xml_diff>